<commit_message>
working for trading timeframe. showing put and call only
</commit_message>
<xml_diff>
--- a/options_vis.xlsx
+++ b/options_vis.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emilfunke/Documents/privat/trading/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emilfunke/PycharmProjects/optionvis/options-visualization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BAA8AA6-7C2E-1947-82BD-26E287C49366}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7620D2D-B2CB-6E49-B1DA-47D5B1DA926B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{50294CAD-143B-4E5F-BF25-ED2866741435}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="109">
   <si>
     <t>DAX</t>
   </si>
@@ -51,9 +51,6 @@
     <t>Opening</t>
   </si>
   <si>
-    <t>Kurs</t>
-  </si>
-  <si>
     <t>Einnahme</t>
   </si>
   <si>
@@ -361,6 +358,12 @@
   </si>
   <si>
     <t>Datum Kauf</t>
+  </si>
+  <si>
+    <t>Kurs VK</t>
+  </si>
+  <si>
+    <t>Kurs EK</t>
   </si>
 </sst>
 </file>
@@ -801,9 +804,9 @@
   <dimension ref="A1:Q118"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A24" sqref="A24"/>
-      <selection pane="bottomLeft" activeCell="D98" sqref="D98"/>
+      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -816,7 +819,7 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -828,40 +831,40 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="37" t="s">
+        <v>106</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="37" t="s">
-        <v>107</v>
-      </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="L1" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L1" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="P1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Q1" s="1"/>
     </row>
@@ -876,10 +879,10 @@
         <v>19.7</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F2" s="5">
         <v>1</v>
@@ -923,7 +926,7 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="29">
-        <v>43696</v>
+        <v>43706</v>
       </c>
       <c r="B3" s="5">
         <v>11800</v>
@@ -932,10 +935,10 @@
         <v>19.7</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F3" s="5">
         <v>1</v>
@@ -987,10 +990,10 @@
         <v>15.8</v>
       </c>
       <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="15" t="s">
         <v>14</v>
-      </c>
-      <c r="E4" s="15" t="s">
-        <v>15</v>
       </c>
       <c r="F4">
         <v>1</v>
@@ -1043,10 +1046,10 @@
         <v>15.8</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -1098,10 +1101,10 @@
         <v>15.4</v>
       </c>
       <c r="D6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="16" t="s">
         <v>19</v>
-      </c>
-      <c r="E6" s="16" t="s">
-        <v>20</v>
       </c>
       <c r="F6" s="5">
         <v>1</v>
@@ -1154,10 +1157,10 @@
         <v>15.4</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F7" s="5">
         <v>1</v>
@@ -1210,10 +1213,10 @@
         <v>13.9</v>
       </c>
       <c r="D8" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="18" t="s">
         <v>22</v>
-      </c>
-      <c r="E8" s="18" t="s">
-        <v>23</v>
       </c>
       <c r="F8" s="17">
         <v>1</v>
@@ -1266,10 +1269,10 @@
         <v>13.9</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F9" s="17">
         <v>1</v>
@@ -1322,10 +1325,10 @@
         <v>13.9</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F10" s="17">
         <v>1</v>
@@ -1377,10 +1380,10 @@
         <v>12.9</v>
       </c>
       <c r="D11" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="16" t="s">
         <v>25</v>
-      </c>
-      <c r="E11" s="16" t="s">
-        <v>26</v>
       </c>
       <c r="F11" s="5">
         <v>1</v>
@@ -1433,10 +1436,10 @@
         <v>12.9</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F12" s="5">
         <v>1</v>
@@ -1489,10 +1492,10 @@
         <v>15.8</v>
       </c>
       <c r="D13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E13" s="27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F13">
         <v>1</v>
@@ -1545,10 +1548,10 @@
         <v>15.8</v>
       </c>
       <c r="D14" s="24" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E14" s="27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F14" s="24">
         <v>1</v>
@@ -1600,10 +1603,10 @@
         <v>15</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E15" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F15" s="5">
         <v>1</v>
@@ -1656,10 +1659,10 @@
         <v>15</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E16" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F16" s="5">
         <v>1</v>
@@ -1712,10 +1715,10 @@
         <v>26</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E17" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F17" s="5">
         <v>1</v>
@@ -1768,10 +1771,10 @@
         <v>24</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E18" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F18" s="5">
         <v>1</v>
@@ -1824,10 +1827,10 @@
         <v>32</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E19" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F19" s="5">
         <v>1</v>
@@ -1879,10 +1882,10 @@
         <v>68</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E20" s="18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F20" s="17">
         <v>1</v>
@@ -1934,10 +1937,10 @@
         <v>35</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E21" s="16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F21" s="5">
         <v>1</v>
@@ -1990,10 +1993,10 @@
         <v>35</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E22" s="16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F22" s="5">
         <v>1</v>
@@ -2046,10 +2049,10 @@
         <v>32</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E23" s="16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F23" s="5">
         <v>1</v>
@@ -2102,10 +2105,10 @@
         <v>33</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E24" s="16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F24" s="5">
         <v>1</v>
@@ -2158,10 +2161,10 @@
         <v>38</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E25" s="16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F25" s="5">
         <v>1</v>
@@ -2214,10 +2217,10 @@
         <v>38</v>
       </c>
       <c r="D26" s="17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E26" s="18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F26" s="17">
         <v>1</v>
@@ -2270,10 +2273,10 @@
         <v>38</v>
       </c>
       <c r="D27" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E27" s="18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F27" s="17">
         <v>1</v>
@@ -2326,10 +2329,10 @@
         <v>31</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E28" s="16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F28" s="5">
         <v>1</v>
@@ -2382,10 +2385,10 @@
         <v>31</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E29" s="16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F29" s="5">
         <v>1</v>
@@ -2438,10 +2441,10 @@
         <v>27</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E30" s="16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F30" s="5">
         <v>1</v>
@@ -2494,10 +2497,10 @@
         <v>24</v>
       </c>
       <c r="D31" s="17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E31" s="18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F31" s="17">
         <v>1</v>
@@ -2549,10 +2552,10 @@
         <v>24</v>
       </c>
       <c r="D32" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="E32" s="18" t="s">
         <v>47</v>
-      </c>
-      <c r="E32" s="18" t="s">
-        <v>48</v>
       </c>
       <c r="F32" s="17">
         <v>1</v>
@@ -2605,10 +2608,10 @@
         <v>23</v>
       </c>
       <c r="D33" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E33" s="16" t="s">
         <v>49</v>
-      </c>
-      <c r="E33" s="16" t="s">
-        <v>50</v>
       </c>
       <c r="F33" s="5">
         <v>1</v>
@@ -2661,10 +2664,10 @@
         <v>31</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E34" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F34" s="5">
         <v>1</v>
@@ -2716,10 +2719,10 @@
         <v>25</v>
       </c>
       <c r="D35" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="E35" s="18" t="s">
         <v>52</v>
-      </c>
-      <c r="E35" s="18" t="s">
-        <v>53</v>
       </c>
       <c r="F35" s="17">
         <v>1</v>
@@ -2772,10 +2775,10 @@
         <v>25</v>
       </c>
       <c r="D36" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E36" s="18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F36" s="17">
         <v>1</v>
@@ -2828,10 +2831,10 @@
         <v>27</v>
       </c>
       <c r="D37" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E37" s="18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F37" s="17">
         <v>1</v>
@@ -2884,10 +2887,10 @@
         <v>30</v>
       </c>
       <c r="D38" s="17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E38" s="18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F38" s="17">
         <v>1</v>
@@ -2921,11 +2924,11 @@
         <v>18990</v>
       </c>
       <c r="O38" s="36">
-        <f t="shared" ref="O38:O94" si="22">O37+M38</f>
+        <f t="shared" ref="O38:O91" si="22">O37+M38</f>
         <v>-2444.6500000000015</v>
       </c>
       <c r="P38" s="33">
-        <f t="shared" ref="P38:P94" si="23">G38-K38</f>
+        <f t="shared" ref="P38:P91" si="23">G38-K38</f>
         <v>102</v>
       </c>
     </row>
@@ -2936,10 +2939,10 @@
       <c r="B39" s="17"/>
       <c r="C39" s="17"/>
       <c r="D39" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E39" s="18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F39" s="17">
         <v>1</v>
@@ -2987,10 +2990,10 @@
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
       <c r="D40" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E40" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F40" s="5">
         <v>1</v>
@@ -3038,10 +3041,10 @@
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
       <c r="D41" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E41" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F41" s="5">
         <v>1</v>
@@ -3089,10 +3092,10 @@
       <c r="B42" s="17"/>
       <c r="C42" s="17"/>
       <c r="D42" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E42" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F42" s="17">
         <v>1</v>
@@ -3141,10 +3144,10 @@
       <c r="B43" s="17"/>
       <c r="C43" s="17"/>
       <c r="D43" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="E43" s="18" t="s">
         <v>59</v>
-      </c>
-      <c r="E43" s="18" t="s">
-        <v>60</v>
       </c>
       <c r="F43" s="17">
         <v>1</v>
@@ -3193,10 +3196,10 @@
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
       <c r="D44" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E44" s="16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F44" s="5">
         <v>1</v>
@@ -3245,10 +3248,10 @@
       <c r="B45" s="5"/>
       <c r="C45" s="5"/>
       <c r="D45" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E45" s="16" t="s">
         <v>62</v>
-      </c>
-      <c r="E45" s="16" t="s">
-        <v>63</v>
       </c>
       <c r="F45" s="5">
         <v>1</v>
@@ -3295,10 +3298,10 @@
       <c r="B46" s="5"/>
       <c r="C46" s="5"/>
       <c r="D46" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E46" s="16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F46" s="5">
         <v>1</v>
@@ -3345,10 +3348,10 @@
       <c r="B47" s="17"/>
       <c r="C47" s="17"/>
       <c r="D47" s="17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E47" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F47" s="17">
         <v>1</v>
@@ -3396,10 +3399,10 @@
       <c r="B48" s="17"/>
       <c r="C48" s="17"/>
       <c r="D48" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E48" s="18" t="s">
         <v>65</v>
-      </c>
-      <c r="E48" s="18" t="s">
-        <v>66</v>
       </c>
       <c r="F48" s="17">
         <v>1</v>
@@ -3447,10 +3450,10 @@
       <c r="B49" s="5"/>
       <c r="C49" s="5"/>
       <c r="D49" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E49" s="16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F49" s="5">
         <v>1</v>
@@ -3499,10 +3502,10 @@
       <c r="B50" s="5"/>
       <c r="C50" s="5"/>
       <c r="D50" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E50" s="16" t="s">
         <v>68</v>
-      </c>
-      <c r="E50" s="16" t="s">
-        <v>69</v>
       </c>
       <c r="F50" s="5">
         <v>1</v>
@@ -3551,10 +3554,10 @@
       <c r="B51" s="5"/>
       <c r="C51" s="5"/>
       <c r="D51" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E51" s="16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F51" s="5">
         <v>1</v>
@@ -3603,10 +3606,10 @@
       <c r="B52" s="17"/>
       <c r="C52" s="17"/>
       <c r="D52" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="E52" s="18" t="s">
         <v>70</v>
-      </c>
-      <c r="E52" s="18" t="s">
-        <v>71</v>
       </c>
       <c r="F52" s="17">
         <v>1</v>
@@ -3655,10 +3658,10 @@
       <c r="B53" s="17"/>
       <c r="C53" s="17"/>
       <c r="D53" s="17" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E53" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F53" s="17">
         <v>1</v>
@@ -3707,10 +3710,10 @@
       <c r="B54" s="5"/>
       <c r="C54" s="5"/>
       <c r="D54" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E54" s="16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F54" s="5">
         <v>1</v>
@@ -3758,10 +3761,10 @@
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
       <c r="D55" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E55" s="16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F55" s="5">
         <v>1</v>
@@ -3809,10 +3812,10 @@
       <c r="B56" s="17"/>
       <c r="C56" s="17"/>
       <c r="D56" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="E56" s="18" t="s">
         <v>74</v>
-      </c>
-      <c r="E56" s="18" t="s">
-        <v>75</v>
       </c>
       <c r="F56" s="17">
         <v>1</v>
@@ -3861,10 +3864,10 @@
       <c r="B57" s="17"/>
       <c r="C57" s="17"/>
       <c r="D57" s="17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E57" s="18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F57" s="17">
         <v>1</v>
@@ -3912,10 +3915,10 @@
       <c r="B58" s="5"/>
       <c r="C58" s="5"/>
       <c r="D58" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E58" s="16" t="s">
         <v>77</v>
-      </c>
-      <c r="E58" s="16" t="s">
-        <v>78</v>
       </c>
       <c r="F58" s="5">
         <v>1</v>
@@ -3963,10 +3966,10 @@
       <c r="B59" s="5"/>
       <c r="C59" s="5"/>
       <c r="D59" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E59" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F59" s="5">
         <v>1</v>
@@ -4014,10 +4017,10 @@
       <c r="B60" s="17"/>
       <c r="C60" s="17"/>
       <c r="D60" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="E60" s="18" t="s">
         <v>79</v>
-      </c>
-      <c r="E60" s="18" t="s">
-        <v>80</v>
       </c>
       <c r="F60" s="17">
         <v>1</v>
@@ -4065,10 +4068,10 @@
       <c r="B61" s="17"/>
       <c r="C61" s="17"/>
       <c r="D61" s="17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E61" s="18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F61" s="17">
         <v>1</v>
@@ -4116,10 +4119,10 @@
       <c r="B62" s="5"/>
       <c r="C62" s="5"/>
       <c r="D62" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="E62" s="16" t="s">
         <v>86</v>
-      </c>
-      <c r="E62" s="16" t="s">
-        <v>87</v>
       </c>
       <c r="F62" s="5">
         <v>1</v>
@@ -4165,10 +4168,10 @@
       <c r="B63" s="5"/>
       <c r="C63" s="5"/>
       <c r="D63" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E63" s="16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F63" s="5">
         <v>1</v>
@@ -4217,10 +4220,10 @@
       <c r="B64" s="5"/>
       <c r="C64" s="5"/>
       <c r="D64" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E64" s="16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F64" s="5">
         <v>1</v>
@@ -4268,10 +4271,10 @@
       <c r="B65" s="17"/>
       <c r="C65" s="17"/>
       <c r="D65" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="E65" s="18" t="s">
         <v>88</v>
-      </c>
-      <c r="E65" s="18" t="s">
-        <v>89</v>
       </c>
       <c r="F65" s="17">
         <v>1</v>
@@ -4319,10 +4322,10 @@
       <c r="B66" s="17"/>
       <c r="C66" s="17"/>
       <c r="D66" s="17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E66" s="18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F66" s="17">
         <v>1</v>
@@ -4371,10 +4374,10 @@
       <c r="B67" s="5"/>
       <c r="C67" s="5"/>
       <c r="D67" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="E67" s="16" t="s">
         <v>90</v>
-      </c>
-      <c r="E67" s="16" t="s">
-        <v>91</v>
       </c>
       <c r="F67" s="5">
         <v>1</v>
@@ -4404,7 +4407,7 @@
         <v>438</v>
       </c>
       <c r="N67" s="7">
-        <f t="shared" ref="N67:N93" si="30">B67*C67*5*F67/100</f>
+        <f t="shared" ref="N67:N91" si="30">B67*C67*5*F67/100</f>
         <v>0</v>
       </c>
       <c r="O67" s="8">
@@ -4423,10 +4426,10 @@
       <c r="B68" s="5"/>
       <c r="C68" s="5"/>
       <c r="D68" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E68" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F68" s="5">
         <v>1</v>
@@ -4474,10 +4477,10 @@
       <c r="B69" s="5"/>
       <c r="C69" s="5"/>
       <c r="D69" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="E69" s="16" t="s">
         <v>90</v>
-      </c>
-      <c r="E69" s="16" t="s">
-        <v>91</v>
       </c>
       <c r="F69" s="5">
         <v>1</v>
@@ -4525,10 +4528,10 @@
       <c r="B70" s="17"/>
       <c r="C70" s="17"/>
       <c r="D70" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="E70" s="18" t="s">
         <v>93</v>
-      </c>
-      <c r="E70" s="18" t="s">
-        <v>94</v>
       </c>
       <c r="F70" s="17">
         <v>1</v>
@@ -4576,10 +4579,10 @@
       <c r="B71" s="17"/>
       <c r="C71" s="17"/>
       <c r="D71" s="17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E71" s="18" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F71" s="17">
         <v>1</v>
@@ -4627,10 +4630,10 @@
       <c r="B72" s="5"/>
       <c r="C72" s="5"/>
       <c r="D72" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E72" s="16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F72" s="5">
         <v>1</v>
@@ -4678,10 +4681,10 @@
       <c r="B73" s="5"/>
       <c r="C73" s="5"/>
       <c r="D73" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E73" s="16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F73" s="5">
         <v>1</v>
@@ -4729,10 +4732,10 @@
       <c r="B74" s="17"/>
       <c r="C74" s="17"/>
       <c r="D74" s="17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E74" s="18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F74" s="17">
         <v>1</v>
@@ -4781,10 +4784,10 @@
       <c r="B75" s="17"/>
       <c r="C75" s="17"/>
       <c r="D75" s="17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E75" s="18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F75" s="17">
         <v>1</v>
@@ -4833,10 +4836,10 @@
       <c r="B76" s="17"/>
       <c r="C76" s="17"/>
       <c r="D76" s="17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E76" s="18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F76" s="17">
         <v>1</v>
@@ -4884,10 +4887,10 @@
       <c r="B77" s="17"/>
       <c r="C77" s="17"/>
       <c r="D77" s="17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E77" s="18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F77" s="17">
         <v>1</v>
@@ -4935,10 +4938,10 @@
       <c r="B78" s="17"/>
       <c r="C78" s="17"/>
       <c r="D78" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E78" s="18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F78" s="17">
         <v>1</v>
@@ -4986,10 +4989,10 @@
       <c r="B79" s="5"/>
       <c r="C79" s="5"/>
       <c r="D79" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E79" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F79" s="5">
         <v>1</v>
@@ -5037,10 +5040,10 @@
       <c r="B80" s="5"/>
       <c r="C80" s="5"/>
       <c r="D80" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E80" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F80" s="5">
         <v>1</v>
@@ -5088,10 +5091,10 @@
       <c r="B81" s="5"/>
       <c r="C81" s="5"/>
       <c r="D81" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="E81" s="16" t="s">
         <v>98</v>
-      </c>
-      <c r="E81" s="16" t="s">
-        <v>99</v>
       </c>
       <c r="F81" s="5">
         <v>1</v>
@@ -5139,10 +5142,10 @@
       <c r="B82" s="17"/>
       <c r="C82" s="17"/>
       <c r="D82" s="17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E82" s="18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F82" s="17">
         <v>1</v>
@@ -5190,10 +5193,10 @@
       <c r="B83" s="17"/>
       <c r="C83" s="17"/>
       <c r="D83" s="17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E83" s="18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F83" s="17">
         <v>1</v>
@@ -5241,10 +5244,10 @@
       <c r="B84" s="17"/>
       <c r="C84" s="17"/>
       <c r="D84" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="E84" s="18" t="s">
         <v>100</v>
-      </c>
-      <c r="E84" s="18" t="s">
-        <v>101</v>
       </c>
       <c r="F84" s="17">
         <v>1</v>
@@ -5292,10 +5295,10 @@
       <c r="B85" s="5"/>
       <c r="C85" s="5"/>
       <c r="D85" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="E85" s="16" t="s">
         <v>102</v>
-      </c>
-      <c r="E85" s="16" t="s">
-        <v>103</v>
       </c>
       <c r="F85" s="5">
         <v>1</v>
@@ -5344,10 +5347,10 @@
       <c r="B86" s="5"/>
       <c r="C86" s="5"/>
       <c r="D86" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E86" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F86" s="5">
         <v>1</v>
@@ -5395,10 +5398,10 @@
       <c r="B87" s="5"/>
       <c r="C87" s="5"/>
       <c r="D87" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E87" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F87" s="5">
         <v>1</v>
@@ -5447,10 +5450,10 @@
       <c r="B88" s="17"/>
       <c r="C88" s="17"/>
       <c r="D88" s="17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E88" s="18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F88" s="17">
         <v>1</v>
@@ -5499,10 +5502,10 @@
       <c r="B89" s="17"/>
       <c r="C89" s="17"/>
       <c r="D89" s="17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E89" s="18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F89" s="17">
         <v>1</v>
@@ -5550,10 +5553,10 @@
       <c r="B90" s="17"/>
       <c r="C90" s="17"/>
       <c r="D90" s="17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E90" s="18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F90" s="17">
         <v>1</v>
@@ -5578,7 +5581,7 @@
         <v>26</v>
       </c>
       <c r="M90" s="33">
-        <f t="shared" ref="M90:M94" si="31">H90-L90</f>
+        <f t="shared" ref="M90:M91" si="31">H90-L90</f>
         <v>-26</v>
       </c>
       <c r="N90" s="9">
@@ -5601,10 +5604,10 @@
       <c r="B91" s="17"/>
       <c r="C91" s="17"/>
       <c r="D91" s="17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E91" s="18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F91" s="17">
         <v>1</v>

</xml_diff>